<commit_message>
Data driven test code
</commit_message>
<xml_diff>
--- a/Selenium-Practice/testData/Datadriventestdata.xlsx
+++ b/Selenium-Practice/testData/Datadriventestdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <t>firstname</t>
   </si>
@@ -39,9 +39,6 @@
     <t>zipcode</t>
   </si>
   <si>
-    <t>emailaddress</t>
-  </si>
-  <si>
     <t>Tom</t>
   </si>
   <si>
@@ -61,6 +58,45 @@
   </si>
   <si>
     <t>tom@gmail.com</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Jill</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Bond</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>jones</t>
+  </si>
+  <si>
+    <t>jack@gmail.com</t>
+  </si>
+  <si>
+    <t>jill@gmail.com</t>
+  </si>
+  <si>
+    <t>james@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -119,9 +155,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
@@ -426,82 +461,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>9876543210</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <v>123456</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>9876542322</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2">
-        <v>9876543210</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
+      <c r="I3">
+        <v>123456</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>9876542223</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4">
+        <v>123456</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>9876543233</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>123456</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>